<commit_message>
refactor: Improved implementation of validation for upload file.
</commit_message>
<xml_diff>
--- a/templates/uploads/leave_requests.xlsx
+++ b/templates/uploads/leave_requests.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EBC\Desktop\payroll-hr\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EBC\Desktop\payroll-hr\templates\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="leave_requests" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -53,7 +53,7 @@
     <t>Recovery</t>
   </si>
   <si>
-    <t>N</t>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -393,7 +393,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>